<commit_message>
Adding logs to the extent report with BasePage and pages
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/master.xlsx
+++ b/src/test/resources/testdata/master.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t xml:space="preserve">TestCases</t>
   </si>
@@ -241,13 +241,14 @@
   </sheetPr>
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="8.53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.65"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="2" style="0" width="8.53"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -290,10 +291,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -350,27 +351,41 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="1"/>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>4</v>
-      </c>
+      <c r="B6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="B7" s="0" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B9" s="0" t="s">
         <v>11</v>
       </c>
     </row>
@@ -378,6 +393,7 @@
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="trainer@way2automation.com"/>
     <hyperlink ref="B4" r:id="rId2" display="java@way2automation.com"/>
+    <hyperlink ref="B5" r:id="rId3" display="trainer@way2automation.com"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
Adding more Business Page Objects and Test Cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata/master.xlsx
+++ b/src/test/resources/testdata/master.xlsx
@@ -38,34 +38,34 @@
     <t xml:space="preserve">ValidateCRMTest</t>
   </si>
   <si>
+    <t xml:space="preserve">username</t>
+  </si>
+  <si>
+    <t xml:space="preserve">password</t>
+  </si>
+  <si>
+    <t xml:space="preserve">browser</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trainer@way2automation.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">askjdfhjskfs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chrome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">java@way2automation.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kjasdhfksdf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firefox</t>
+  </si>
+  <si>
     <t xml:space="preserve">N</t>
-  </si>
-  <si>
-    <t xml:space="preserve">username</t>
-  </si>
-  <si>
-    <t xml:space="preserve">password</t>
-  </si>
-  <si>
-    <t xml:space="preserve">browser</t>
-  </si>
-  <si>
-    <t xml:space="preserve">trainer@way2automation.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">askjdfhjskfs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">chrome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">java@way2automation.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">kjasdhfksdf</t>
-  </si>
-  <si>
-    <t xml:space="preserve">firefox</t>
   </si>
 </sst>
 </file>
@@ -272,7 +272,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -291,10 +291,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -314,13 +314,13 @@
         <v>1</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="0" t="s">
+      <c r="D2" s="0" t="s">
         <v>7</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -328,13 +328,13 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -342,27 +342,27 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="0" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>13</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" s="0" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -378,17 +378,18 @@
         <v>1</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>11</v>
-      </c>
-    </row>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B3" r:id="rId1" display="trainer@way2automation.com"/>

</xml_diff>